<commit_message>
Finalize project structure, README, UI polish and bug fixes
</commit_message>
<xml_diff>
--- a/backend/data/weekly_schedule.xlsx
+++ b/backend/data/weekly_schedule.xlsx
@@ -420,7 +420,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-11-16</v>
+        <v>2025-11-23</v>
       </c>
       <c r="B2" t="str">
         <v>8:00-16:00</v>
@@ -431,7 +431,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-11-16</v>
+        <v>2025-11-23</v>
       </c>
       <c r="B3" t="str">
         <v>16:00-00:00</v>
@@ -442,7 +442,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-11-17</v>
+        <v>2025-11-24</v>
       </c>
       <c r="B4" t="str">
         <v>8:00-16:00</v>
@@ -453,123 +453,123 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2025-11-17</v>
+        <v>2025-11-24</v>
       </c>
       <c r="B5" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C5" t="str">
-        <v>Anton Iosifov, Haim Kuper</v>
+        <v>Harry Potter, Anton Iosifov</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2025-11-18</v>
+        <v>2025-11-25</v>
       </c>
       <c r="B6" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C6" t="str">
-        <v>Yaniv Arad, John Snow</v>
+        <v>Yaniv Arad, Haim Kuper</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2025-11-18</v>
+        <v>2025-11-25</v>
       </c>
       <c r="B7" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C7" t="str">
-        <v>Alla Khrol, Spider Man</v>
+        <v>John Snow, Alla Khrol</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2025-11-19</v>
+        <v>2025-11-26</v>
       </c>
       <c r="B8" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C8" t="str">
-        <v>Anton Iosifov, Haim Kuper</v>
+        <v>Spider Man, Harry Potter</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2025-11-19</v>
+        <v>2025-11-26</v>
       </c>
       <c r="B9" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C9" t="str">
-        <v>Yaniv Arad, John Snow</v>
+        <v>Anton Iosifov, Yaniv Arad</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2025-11-20</v>
+        <v>2025-11-27</v>
       </c>
       <c r="B10" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C10" t="str">
-        <v>Alla Khrol, Spider Man</v>
+        <v>Haim Kuper, John Snow</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2025-11-20</v>
+        <v>2025-11-27</v>
       </c>
       <c r="B11" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C11" t="str">
-        <v>Anton Iosifov, Haim Kuper</v>
+        <v>Alla Khrol, Spider Man</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2025-11-21</v>
+        <v>2025-11-28</v>
       </c>
       <c r="B12" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C12" t="str">
-        <v>Yaniv Arad, John Snow</v>
+        <v>Harry Potter, Anton Iosifov</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2025-11-21</v>
+        <v>2025-11-28</v>
       </c>
       <c r="B13" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C13" t="str">
-        <v>Alla Khrol, Spider Man</v>
+        <v>Yaniv Arad, Haim Kuper</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2025-11-22</v>
+        <v>2025-11-29</v>
       </c>
       <c r="B14" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C14" t="str">
-        <v>Anton Iosifov, Haim Kuper</v>
+        <v>John Snow, Alla Khrol</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2025-11-22</v>
+        <v>2025-11-29</v>
       </c>
       <c r="B15" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C15" t="str">
-        <v>Yaniv Arad, John Snow</v>
+        <v>Spider Man, Harry Potter</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: migrate to React + TypeScript frontend, backend updates
</commit_message>
<xml_diff>
--- a/backend/data/weekly_schedule.xlsx
+++ b/backend/data/weekly_schedule.xlsx
@@ -420,156 +420,156 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-11-23</v>
+        <v>2025-12-07</v>
       </c>
       <c r="B2" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C2" t="str">
-        <v>Anton Iosifov, Yaniv Arad</v>
+        <v>Anton Iosifov, David Cohen</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-11-23</v>
+        <v>2025-12-07</v>
       </c>
       <c r="B3" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C3" t="str">
-        <v>Haim Kuper, John Snow</v>
+        <v>Marina Levi, Alex Brown</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-11-24</v>
+        <v>2025-12-08</v>
       </c>
       <c r="B4" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C4" t="str">
-        <v>Alla Khrol, Spider Man</v>
+        <v>Tommy Gun, Tony Saprano</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2025-11-24</v>
+        <v>2025-12-08</v>
       </c>
       <c r="B5" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C5" t="str">
-        <v>Harry Potter, Anton Iosifov</v>
+        <v>Anton Iosifov, Marina Levi</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2025-11-25</v>
+        <v>2025-12-09</v>
       </c>
       <c r="B6" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C6" t="str">
-        <v>Yaniv Arad, Haim Kuper</v>
+        <v>David Cohen, Alex Brown</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2025-11-25</v>
+        <v>2025-12-09</v>
       </c>
       <c r="B7" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C7" t="str">
-        <v>John Snow, Alla Khrol</v>
+        <v>Tommy Gun, Tony Saprano</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>2025-11-26</v>
+        <v>2025-12-10</v>
       </c>
       <c r="B8" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C8" t="str">
-        <v>Spider Man, Harry Potter</v>
+        <v>Anton Iosifov, Marina Levi</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>2025-11-26</v>
+        <v>2025-12-10</v>
       </c>
       <c r="B9" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C9" t="str">
-        <v>Anton Iosifov, Yaniv Arad</v>
+        <v>David Cohen, Alex Brown</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>2025-11-27</v>
+        <v>2025-12-11</v>
       </c>
       <c r="B10" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C10" t="str">
-        <v>Haim Kuper, John Snow</v>
+        <v>Tommy Gun, Tony Saprano</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>2025-11-27</v>
+        <v>2025-12-11</v>
       </c>
       <c r="B11" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C11" t="str">
-        <v>Alla Khrol, Spider Man</v>
+        <v>Anton Iosifov, Marina Levi</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>2025-11-28</v>
+        <v>2025-12-12</v>
       </c>
       <c r="B12" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C12" t="str">
-        <v>Harry Potter, Anton Iosifov</v>
+        <v>David Cohen, Alex Brown</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>2025-11-28</v>
+        <v>2025-12-12</v>
       </c>
       <c r="B13" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C13" t="str">
-        <v>Yaniv Arad, Haim Kuper</v>
+        <v>Tommy Gun, Tony Saprano</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>2025-11-29</v>
+        <v>2025-12-13</v>
       </c>
       <c r="B14" t="str">
         <v>8:00-16:00</v>
       </c>
       <c r="C14" t="str">
-        <v>John Snow, Alla Khrol</v>
+        <v>Anton Iosifov, Marina Levi</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>2025-11-29</v>
+        <v>2025-12-13</v>
       </c>
       <c r="B15" t="str">
         <v>16:00-00:00</v>
       </c>
       <c r="C15" t="str">
-        <v>Spider Man, Harry Potter</v>
+        <v>David Cohen, Alex Brown</v>
       </c>
     </row>
   </sheetData>

</xml_diff>